<commit_message>
heterogeneity and other project level modifications
</commit_message>
<xml_diff>
--- a/results/careless_response_proportions.xlsx
+++ b/results/careless_response_proportions.xlsx
@@ -7,14 +7,14 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="cr_proportions_total" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="cr_proportions_by_year" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="cr_proportions_by_journal" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="cr_proportions_by_sample_source" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="cr_proportions_by_sample_method" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="cr_proportions_by_sample_plat" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="cr_proportions_by_method" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="cr_proportions_by_method_type" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="proportions_total" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="proportions_year" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="proportions_journal" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="proportions_sample_source" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="proportions_sample_method" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="proportions_platform" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="proportions_cr_method" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="proportions_cr_type" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -458,7 +458,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>cr_proportion_total</t>
+          <t>proportions_total</t>
         </is>
       </c>
     </row>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>cr_proportion_year</t>
+          <t>proportions_year</t>
         </is>
       </c>
     </row>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>cr_proportion_journal</t>
+          <t>proportions_journal</t>
         </is>
       </c>
     </row>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>cr_proportion_source</t>
+          <t>proportions_sample_source</t>
         </is>
       </c>
     </row>
@@ -5069,7 +5069,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>cr_proportion_method</t>
+          <t>proportions_sample_method</t>
         </is>
       </c>
     </row>
@@ -6418,7 +6418,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>cr_proportion_platform</t>
+          <t>proportions_platform</t>
         </is>
       </c>
     </row>
@@ -7376,7 +7376,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>cr_proportion</t>
+          <t>proportions_cr_method</t>
         </is>
       </c>
     </row>
@@ -9022,7 +9022,7 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>cr_proportion</t>
+          <t>proportions_cr_type</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
export frequencies to workbook
</commit_message>
<xml_diff>
--- a/results/careless_response_proportions.xlsx
+++ b/results/careless_response_proportions.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="proportions_total" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="proportions_year" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="proportions_journal" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="proportions_sample_source" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="proportions_sample_method" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="proportions_platform" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="proportions_cr_method" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="proportions_cr_type" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="proportions_total" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="proportions_year" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="proportions_journal" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="proportions_sample_source" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="proportions_sample_method" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="proportions_platform" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="proportions_cr_method" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="proportions_cr_type" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>